<commit_message>
Updates to Upload and Edit
Resource Upload and Edit changes, DBML changes, timesheet
</commit_message>
<xml_diff>
--- a/Timesheets/Timesheet - Riaan.xlsx
+++ b/Timesheets/Timesheet - Riaan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="39">
   <si>
     <t>Person</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Resource Upload changes</t>
+  </si>
+  <si>
+    <t>Resource Edit</t>
+  </si>
+  <si>
+    <t>Resource Upload changes and Resource Edit</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1009,7 @@
   <dimension ref="A2:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,10 +1147,32 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4">
+        <v>41653</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4">
+        <v>41655</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>4.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -1170,7 +1198,7 @@
       </c>
       <c r="C20">
         <f>SUM(C4:C18)</f>
-        <v>36</v>
+        <v>45.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to get shit working
ASDjalgf
</commit_message>
<xml_diff>
--- a/Timesheets/Timesheet - Riaan.xlsx
+++ b/Timesheets/Timesheet - Riaan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
   <si>
     <t>Person</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Resource Upload changes and Resource Edit</t>
+  </si>
+  <si>
+    <t>Resource View &amp; Listings</t>
+  </si>
+  <si>
+    <t>ResourceView, Listings, Uploads &amp; Search</t>
   </si>
 </sst>
 </file>
@@ -493,7 +499,7 @@
   <dimension ref="A2:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +757,7 @@
   <dimension ref="A2:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1015,7 @@
   <dimension ref="A2:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,13 +1181,46 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4">
+        <v>41656</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>4.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4">
+        <v>41657</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="4">
+        <v>41658</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1198,7 +1237,7 @@
       </c>
       <c r="C20">
         <f>SUM(C4:C18)</f>
-        <v>45.5</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>